<commit_message>
one test case broke into many test cases as per pages
</commit_message>
<xml_diff>
--- a/src/main/java/com/amt/testData/NewTestData.xlsx
+++ b/src/main/java/com/amt/testData/NewTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="OutrightBCHwithoutMaintenanceEd" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="72">
   <si>
     <t xml:space="preserve">manufacturer</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t xml:space="preserve">main_cost_used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A8</t>
   </si>
   <si>
     <t xml:space="preserve">YES</t>
@@ -375,11 +372,11 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="1" width="24.45"/>
@@ -528,7 +525,7 @@
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
@@ -678,7 +675,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
@@ -835,7 +832,7 @@
       <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -947,7 +944,7 @@
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1041,7 +1038,7 @@
       <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1149,11 +1146,11 @@
   </sheetPr>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
@@ -1229,7 +1226,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0</v>
@@ -1268,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P2" s="1" t="n">
         <v>0.2</v>
@@ -1308,7 +1305,7 @@
       <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1444,7 +1441,7 @@
       <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1580,7 +1577,7 @@
       <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
@@ -1695,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P2" s="1" t="n">
         <v>0.2</v>
@@ -1735,7 +1732,7 @@
       <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.31"/>
@@ -1878,7 +1875,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
@@ -2046,7 +2043,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
@@ -2161,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P2" s="1" t="n">
         <v>0.2</v>
@@ -2201,7 +2198,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2295,7 +2292,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.35"/>
@@ -2323,19 +2320,19 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>58</v>
@@ -2344,7 +2341,7 @@
         <v>60</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,7 +2407,7 @@
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
@@ -2532,7 +2529,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.66"/>
@@ -2714,7 +2711,7 @@
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.66"/>
@@ -2848,7 +2845,7 @@
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3008,7 +3005,7 @@
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
@@ -3158,7 +3155,7 @@
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3318,7 +3315,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>

</xml_diff>

<commit_message>
Re-execution Logic written for failed test cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/amt/testData/NewTestData.xlsx
+++ b/src/main/java/com/amt/testData/NewTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="OutrightBCHwithoutMaintenanceEd" sheetId="1" state="visible" r:id="rId2"/>
@@ -372,11 +372,11 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="1" width="24.45"/>
@@ -482,7 +482,7 @@
         <v>199.99</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>21</v>
@@ -525,7 +525,7 @@
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
@@ -675,7 +675,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
@@ -832,7 +832,7 @@
       <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -944,7 +944,7 @@
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1038,7 +1038,7 @@
       <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1146,11 +1146,11 @@
   </sheetPr>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
@@ -1305,7 +1305,7 @@
       <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1441,7 +1441,7 @@
       <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1577,7 +1577,7 @@
       <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
@@ -1732,7 +1732,7 @@
       <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.31"/>
@@ -1875,7 +1875,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
@@ -2043,7 +2043,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
@@ -2198,7 +2198,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2292,7 +2292,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.35"/>
@@ -2407,7 +2407,7 @@
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
@@ -2529,7 +2529,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.66"/>
@@ -2711,7 +2711,7 @@
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.66"/>
@@ -2845,7 +2845,7 @@
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3005,7 +3005,7 @@
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
@@ -3155,7 +3155,7 @@
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3315,7 +3315,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>

</xml_diff>

<commit_message>
code for broker hpnr added
</commit_message>
<xml_diff>
--- a/src/main/java/com/amt/testData/NewTestData.xlsx
+++ b/src/main/java/com/amt/testData/NewTestData.xlsx
@@ -8,30 +8,31 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="BrokerHPR" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="BrokerCPwithoutMaintenance" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="OutrightBCHwithoutMaintenanceEd" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="BrokerFLwithoutMaintenanceEdit" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="BrokerFLwithoutMaintenance" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="BrokerFLwithMaintenanceEdit" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="BrokerFLwithMaintenance" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="BrokerPCHwithMaintenanceEdit" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="BrokerPCHwithoutMaintenanceEdit" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="BrokerBCHwithMaintenanceEdit" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="xyz" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="BrokerBCHwithoutMaintenanceEdit" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="BrokerPCPwithoutMaintenance" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="BrokerPCHwithMaintenance" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="BrokerPCHwithoutMaintenance" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="BrokerBCHwithMaintenance" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="OutrightFLwithMaintenance" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="OutrightPCHwithoutMaintenance" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="OutrightFLwithoutMaintenance" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="OutrightPCHwithMaintenance" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="OutrightBCHwithoutMaintenance" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="OutrightBCHwithMaintenance" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="BrokerBCHwithoutMaintenance" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="audibrokerHPR" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="BrokerHPNR" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="BrokerHPR" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="BrokerCPwithoutMaintenance" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="OutrightBCHwithoutMaintenanceEd" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="BrokerFLwithoutMaintenanceEdit" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="BrokerFLwithoutMaintenance" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="BrokerFLwithMaintenanceEdit" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="BrokerFLwithMaintenance" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="BrokerPCHwithMaintenanceEdit" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="BrokerPCHwithoutMaintenanceEdit" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="BrokerBCHwithMaintenanceEdit" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="xyz" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="BrokerBCHwithoutMaintenanceEdit" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="BrokerPCPwithoutMaintenance" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="BrokerPCHwithMaintenance" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="BrokerPCHwithoutMaintenance" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="BrokerBCHwithMaintenance" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="OutrightFLwithMaintenance" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="OutrightPCHwithoutMaintenance" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="OutrightFLwithoutMaintenance" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="OutrightPCHwithMaintenance" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="OutrightBCHwithoutMaintenance" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="OutrightBCHwithMaintenance" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="BrokerBCHwithoutMaintenance" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="audibrokerHPR" sheetId="25" state="visible" r:id="rId26"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="73">
   <si>
     <t xml:space="preserve">manufacturer </t>
   </si>
@@ -378,10 +379,10 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
@@ -532,13 +533,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.6"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -572,39 +581,30 @@
         <v>48</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -640,46 +640,37 @@
         <v>1000</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="L2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="O2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="M2" s="1" t="n">
-        <v>400</v>
-      </c>
-      <c r="N2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>3</v>
-      </c>
       <c r="P2" s="1" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="T2" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U2" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -692,20 +683,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.43"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -721,45 +705,57 @@
         <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -777,45 +773,57 @@
         <v>600</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>20000</v>
-      </c>
-      <c r="G2" s="1" t="n">
+        <v>60000</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>44959</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>25000</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>44959</v>
-      </c>
       <c r="L2" s="1" t="n">
-        <v>12</v>
+        <v>2000</v>
       </c>
       <c r="M2" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="n">
         <v>5000</v>
       </c>
-      <c r="N2" s="1" t="n">
+      <c r="R2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="O2" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="U2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -835,20 +843,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -865,48 +872,45 @@
         <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -924,55 +928,52 @@
         <v>600</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>60000</v>
-      </c>
-      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="K2" s="2" t="n">
         <v>44959</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="L2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="M2" s="1" t="n">
         <v>5000</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="N2" s="1" t="n">
         <v>1000</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="N2" s="1" t="n">
-        <v>5000</v>
       </c>
       <c r="O2" s="1" t="n">
         <v>2000</v>
       </c>
       <c r="P2" s="1" t="n">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="S2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -985,17 +986,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,60 +1010,54 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1071,65 +1069,61 @@
         <v>22</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>600</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>60000</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="G2" s="2" t="n">
         <v>44959</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="H2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="I2" s="1" t="n">
         <v>5000</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>3000</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>900</v>
-      </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1" t="n">
+        <v>1000</v>
+      </c>
       <c r="K2" s="1" t="n">
         <v>2000</v>
       </c>
       <c r="L2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="M2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="R2" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>600</v>
-      </c>
-      <c r="T2" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1142,13 +1136,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1158,39 +1157,60 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1201,41 +1221,60 @@
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="E2" s="2" t="n">
         <v>44959</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="F2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="G2" s="1" t="n">
         <v>5000</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="H2" s="1" t="n">
+        <v>3000</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>900</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>400</v>
-      </c>
-      <c r="K2" s="1" t="n">
+      <c r="M2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>60</v>
+      <c r="P2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>600</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1254,13 +1293,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1285,15 +1324,24 @@
         <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1320,15 +1368,24 @@
         <v>1000</v>
       </c>
       <c r="H2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="J2" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="K2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="J2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1348,13 +1405,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1379,24 +1436,15 @@
         <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1423,25 +1471,16 @@
         <v>1000</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>400</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1460,80 +1499,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="25.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1544,65 +1558,47 @@
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0</v>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>44959</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>20000</v>
+        <v>1000</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>6000</v>
+        <v>400</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>199.99</v>
-      </c>
-      <c r="N2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1615,13 +1611,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="25.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1640,42 +1643,48 @@
         <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1696,43 +1705,49 @@
         <v>100</v>
       </c>
       <c r="F2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>20000</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="H2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>10000</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="J2" s="1" t="n">
         <v>6000</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="K2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="L2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="M2" s="1" t="n">
         <v>199.99</v>
       </c>
-      <c r="L2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>60</v>
+      <c r="S2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1753,11 +1768,11 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1868,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1889,13 +1904,13 @@
   </sheetPr>
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
   </cols>
@@ -1929,22 +1944,22 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
@@ -1993,21 +2008,21 @@
       <c r="I2" s="1" t="n">
         <v>900</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="n">
+      <c r="J2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="M2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="N2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="P2" s="1" t="n">
         <v>1</v>
@@ -2044,20 +2059,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="25.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2076,48 +2084,42 @@
         <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>66</v>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2138,49 +2140,43 @@
         <v>100</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>100</v>
+        <v>20000</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>6000</v>
+        <v>1000</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>2000</v>
+        <v>199.99</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>199.99</v>
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="N2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>0.2</v>
+      <c r="O2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2199,18 +2195,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="27.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="25.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -2231,42 +2227,48 @@
         <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2287,43 +2289,49 @@
         <v>100</v>
       </c>
       <c r="F2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>20000</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="H2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>10000</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="J2" s="1" t="n">
         <v>6000</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="K2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="L2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="M2" s="1" t="n">
         <v>199.99</v>
       </c>
-      <c r="L2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>25</v>
+      <c r="S2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2342,18 +2350,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="25.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="27.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -2374,48 +2382,42 @@
         <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>66</v>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2436,48 +2438,42 @@
         <v>100</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>100</v>
+        <v>20000</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>6000</v>
+        <v>1000</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>2000</v>
+        <v>199.99</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>199.99</v>
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="N2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>0.2</v>
+      <c r="O2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2497,46 +2493,80 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="25.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2547,38 +2577,65 @@
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>44959</v>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>5000</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>6000</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="n">
+        <v>199.99</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2591,13 +2648,107 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>44959</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.35"/>
@@ -2706,77 +2857,81 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="1" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="27.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>45</v>
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2788,54 +2943,58 @@
         <v>22</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>600</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>60000</v>
+        <v>1200</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>44959</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>6000</v>
-      </c>
-      <c r="J2" s="1" t="n">
+        <v>900</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="L2" s="1" t="n">
         <v>1000</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>199.99</v>
       </c>
       <c r="M2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>46</v>
+      <c r="N2" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="O2" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>600</v>
+      </c>
+      <c r="T2" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2855,25 +3014,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="1" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="27.69"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2885,57 +3043,48 @@
         <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2955,56 +3104,47 @@
       <c r="E2" s="1" t="n">
         <v>60000</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>44959</v>
+      <c r="F2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>20000</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>12</v>
+        <v>10000</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="J2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="K2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="K2" s="1" t="n">
-        <v>2000</v>
-      </c>
       <c r="L2" s="1" t="n">
-        <v>10</v>
+        <v>199.99</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="N2" s="1" t="n">
-        <v>4</v>
+        <v>100</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="O2" s="1" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="P2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>5000</v>
+        <v>200</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="T2" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U2" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>54</v>
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3023,13 +3163,181 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.6"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>600</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>60000</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>44959</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
@@ -3126,188 +3434,6 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:Y2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="33.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.66"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>600</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>60000</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>44959</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>5000</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>400</v>
-      </c>
-      <c r="N2" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="T2" s="1" t="n">
-        <v>5000</v>
-      </c>
-      <c r="U2" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="V2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="W2" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="X2" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="Y2" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3327,16 +3453,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="33.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="33.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3347,48 +3473,72 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3399,49 +3549,73 @@
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>600</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>60000</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="G2" s="2" t="n">
         <v>44959</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="H2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="I2" s="1" t="n">
         <v>5000</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="J2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="K2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="L2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="M2" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="N2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="O2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="P2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="N2" s="1" t="n">
+      <c r="Q2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O2" s="1" t="n">
+      <c r="R2" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="P2" s="1" t="n">
+      <c r="S2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="T2" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="V2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3461,13 +3635,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="33.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.66"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3477,63 +3655,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3544,65 +3707,50 @@
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>600</v>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>44959</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>60000</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>44959</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>1000</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>400</v>
+        <v>3</v>
       </c>
       <c r="N2" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O2" s="1" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="P2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="Q2" s="1" t="n">
-        <v>5000</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="T2" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U2" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>60</v>
+      <c r="Q2" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -3621,21 +3769,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.6"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3669,30 +3809,39 @@
         <v>48</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3728,37 +3877,46 @@
         <v>1000</v>
       </c>
       <c r="K2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="M2" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="N2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="M2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="N2" s="1" t="n">
+      <c r="O2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="n">
         <v>5000</v>
       </c>
-      <c r="O2" s="1" t="n">
+      <c r="R2" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="P2" s="1" t="n">
+      <c r="S2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="Q2" s="1" t="n">
+      <c r="T2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="R2" s="1" t="n">
+      <c r="U2" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>25</v>
+      <c r="V2" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
created outright hpnr scenario
</commit_message>
<xml_diff>
--- a/src/main/java/com/amt/testData/NewTestData.xlsx
+++ b/src/main/java/com/amt/testData/NewTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="BrokerCPwithMaintenance" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,6 +35,7 @@
     <sheet name="OutrightBCHwithMaintenance" sheetId="25" state="visible" r:id="rId26"/>
     <sheet name="BrokerBCHwithoutMaintenance" sheetId="26" state="visible" r:id="rId27"/>
     <sheet name="audibrokerHPR" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="OutrightHPNRwithoutMaintenance" sheetId="28" state="visible" r:id="rId29"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="90">
   <si>
     <t xml:space="preserve">manufacturer </t>
   </si>
@@ -268,6 +269,54 @@
   </si>
   <si>
     <t xml:space="preserve">commisionvalue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manufacurer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle_Basic_price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">additional_terms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vehicle_profit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maintenance_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matrix_credit_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">security_deposit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balloon_payment_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">part_exchange_actual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">part_exchange_given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">less_finance_settlement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">order_deposit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finance_deposit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document_fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1 Credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP(N) - HP(N),HP,CP,PCP</t>
   </si>
 </sst>
 </file>
@@ -387,7 +436,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.83"/>
@@ -558,7 +607,7 @@
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.66"/>
@@ -692,7 +741,7 @@
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -852,7 +901,7 @@
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
@@ -1002,7 +1051,7 @@
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1162,7 +1211,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
@@ -1305,7 +1354,7 @@
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
@@ -1451,11 +1500,11 @@
   </sheetPr>
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
@@ -1614,7 +1663,7 @@
       <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1726,7 +1775,7 @@
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1820,7 +1869,7 @@
       <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1932,7 +1981,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.83"/>
@@ -2103,7 +2152,7 @@
       <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
@@ -2258,7 +2307,7 @@
       <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2394,7 +2443,7 @@
       <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2530,7 +2579,7 @@
       <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
@@ -2685,7 +2734,7 @@
       <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.31"/>
@@ -2828,7 +2877,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
@@ -2983,7 +3032,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3077,7 +3126,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.35"/>
@@ -3168,6 +3217,157 @@
       </c>
       <c r="M2" s="1" t="n">
         <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="0" width="23.08"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>630</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>22000</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>199.99</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3192,7 +3392,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
@@ -3349,7 +3549,7 @@
       <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
@@ -3506,7 +3706,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
@@ -3663,7 +3863,7 @@
       <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="1" width="24.45"/>
@@ -3812,7 +4012,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
@@ -3980,7 +4180,7 @@
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
@@ -4102,7 +4302,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.66"/>

</xml_diff>

<commit_message>
wrote code for outright hpr with maintenance
</commit_message>
<xml_diff>
--- a/src/main/java/com/amt/testData/NewTestData.xlsx
+++ b/src/main/java/com/amt/testData/NewTestData.xlsx
@@ -8,38 +8,39 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="OutrightHPNRwithMaintenance" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="OutrightPCPwithoutMaintenance" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="OutrightCPwithoutMaintenance" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="OutrightHPRwithoutMaintenance" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="BrokerCPwithMaintenance" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="BrokerPCPwithMaintenance" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="BrokerHPNR" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="BrokerHPR" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="BrokerCPwithoutMaintenance" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="OutrightBCHwithoutMaintenanceEd" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="BrokerFLwithoutMaintenanceEdit" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="BrokerFLwithoutMaintenance" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="BrokerFLwithMaintenanceEdit" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="BrokerFLwithMaintenance" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="BrokerPCHwithMaintenanceEdit" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="BrokerPCHwithoutMaintenanceEdit" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="BrokerBCHwithMaintenanceEdit" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="xyz" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="BrokerBCHwithoutMaintenanceEdit" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="BrokerPCPwithoutMaintenance" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="BrokerPCHwithMaintenance" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="BrokerPCHwithoutMaintenance" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="BrokerBCHwithMaintenance" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="OutrightFLwithMaintenance" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="OutrightPCHwithoutMaintenance" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="OutrightFLwithoutMaintenance" sheetId="26" state="visible" r:id="rId27"/>
-    <sheet name="OutrightPCHwithMaintenance" sheetId="27" state="visible" r:id="rId28"/>
-    <sheet name="OutrightBCHwithoutMaintenance" sheetId="28" state="visible" r:id="rId29"/>
-    <sheet name="OutrightBCHwithMaintenance" sheetId="29" state="visible" r:id="rId30"/>
-    <sheet name="BrokerBCHwithoutMaintenance" sheetId="30" state="visible" r:id="rId31"/>
-    <sheet name="audibrokerHPR" sheetId="31" state="visible" r:id="rId32"/>
-    <sheet name="OutrightHPNRwithoutMaintenance" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="OutrightHPRwithMaintenance" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="OutrightHPNRwithMaintenance" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="OutrightPCPwithoutMaintenance" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="OutrightCPwithoutMaintenance" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="OutrightHPRwithoutMaintenance" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="BrokerCPwithMaintenance" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="BrokerPCPwithMaintenance" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="BrokerHPNR" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="BrokerHPR" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="BrokerCPwithoutMaintenance" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="OutrightBCHwithoutMaintenanceEd" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="BrokerFLwithoutMaintenanceEdit" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="BrokerFLwithoutMaintenance" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="BrokerFLwithMaintenanceEdit" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="BrokerFLwithMaintenance" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="BrokerPCHwithMaintenanceEdit" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="BrokerPCHwithoutMaintenanceEdit" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="BrokerBCHwithMaintenanceEdit" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="xyz" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="BrokerBCHwithoutMaintenanceEdit" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="BrokerPCPwithoutMaintenance" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="BrokerPCHwithMaintenance" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="BrokerPCHwithoutMaintenance" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="BrokerBCHwithMaintenance" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="OutrightFLwithMaintenance" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="OutrightPCHwithoutMaintenance" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="OutrightFLwithoutMaintenance" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="OutrightPCHwithMaintenance" sheetId="28" state="visible" r:id="rId29"/>
+    <sheet name="OutrightBCHwithoutMaintenance" sheetId="29" state="visible" r:id="rId30"/>
+    <sheet name="OutrightBCHwithMaintenance" sheetId="30" state="visible" r:id="rId31"/>
+    <sheet name="BrokerBCHwithoutMaintenance" sheetId="31" state="visible" r:id="rId32"/>
+    <sheet name="audibrokerHPR" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="OutrightHPNRwithoutMaintenance" sheetId="33" state="visible" r:id="rId34"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="97">
   <si>
     <t xml:space="preserve">manufacurer</t>
   </si>
@@ -134,6 +135,9 @@
     <t xml:space="preserve">A1 Credit</t>
   </si>
   <si>
+    <t xml:space="preserve">HirePurchaseRegulated</t>
+  </si>
+  <si>
     <t xml:space="preserve">HirePurchaseNonRegulated</t>
   </si>
   <si>
@@ -147,9 +151,6 @@
   </si>
   <si>
     <t xml:space="preserve">ContractPurchase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HirePurchaseRegulated</t>
   </si>
   <si>
     <t xml:space="preserve">manufacturer </t>
@@ -467,11 +468,11 @@
   </sheetPr>
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W2" activeCellId="0" sqref="W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="3" style="0" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
@@ -635,77 +636,81 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="2" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="27.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>74</v>
+        <v>38</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -717,54 +722,58 @@
         <v>24</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>60000</v>
+        <v>1200</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>44959</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>6000</v>
-      </c>
-      <c r="J2" s="2" t="n">
+        <v>900</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="K2" s="2" t="n">
-        <v>1000</v>
-      </c>
       <c r="L2" s="2" t="n">
-        <v>199.99</v>
+        <v>1000</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>28</v>
+      <c r="N2" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T2" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -784,25 +793,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="2" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="27.69"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -814,57 +822,48 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>52</v>
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="V1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -884,56 +883,47 @@
       <c r="E2" s="2" t="n">
         <v>60000</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>44959</v>
+      <c r="F2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>20000</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>12</v>
+        <v>10000</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>10</v>
+        <v>199.99</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="N2" s="2" t="n">
-        <v>4</v>
+        <v>100</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="2" t="n">
-        <v>5000</v>
+        <v>200</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="R2" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="S2" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="T2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U2" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>82</v>
+        <v>0</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -952,13 +942,181 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.6"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>60000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>44959</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U2" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
@@ -1055,188 +1213,6 @@
         <v>5</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:Y2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="33.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.66"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>60000</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>44959</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="M2" s="2" t="n">
-        <v>400</v>
-      </c>
-      <c r="N2" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="O2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="P2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="R2" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="S2" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="T2" s="2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="U2" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="V2" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="W2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="X2" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="Y2" s="2" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1256,16 +1232,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="33.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="33.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1276,48 +1252,72 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1328,49 +1328,73 @@
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>60000</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="G2" s="3" t="n">
         <v>44959</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="H2" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="I2" s="2" t="n">
         <v>5000</v>
       </c>
-      <c r="G2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H2" s="2" t="n">
+      <c r="J2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="L2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="M2" s="2" t="n">
         <v>400</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="N2" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="n">
+      <c r="O2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="M2" s="2" t="n">
+      <c r="P2" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="N2" s="2" t="n">
+      <c r="Q2" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="R2" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="n">
+      <c r="S2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="T2" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="U2" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="V2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="W2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="X2" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1390,13 +1414,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="33.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.66"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1406,63 +1434,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>50</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="V1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1473,65 +1486,50 @@
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>600</v>
+      <c r="C2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>44959</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>60000</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>44959</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>1000</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>400</v>
+        <v>3</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q2" s="2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="R2" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="S2" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="T2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U2" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>87</v>
+      <c r="Q2" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1550,13 +1548,173 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>60000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>44959</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U2" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
@@ -1695,7 +1853,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1706,7 +1864,7 @@
       <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1841,149 +1999,6 @@
         <v>200</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:R2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.43"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>20000</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>25000</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K2" s="3" t="n">
-        <v>44959</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="M2" s="2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="N2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O2" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="P2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="R2" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2003,20 +2018,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2033,48 +2047,45 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="R1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2092,55 +2103,52 @@
         <v>600</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>60000</v>
-      </c>
-      <c r="F2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>25000</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="K2" s="3" t="n">
         <v>44959</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="L2" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="M2" s="2" t="n">
         <v>5000</v>
       </c>
-      <c r="J2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2" t="n">
-        <v>5</v>
-      </c>
       <c r="N2" s="2" t="n">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="O2" s="2" t="n">
         <v>2000</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="R2" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="S2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2153,15 +2161,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="3" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2181,56 +2190,65 @@
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="T1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="U1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="V1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="W1" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -2239,53 +2257,62 @@
       <c r="D2" s="0" t="n">
         <v>630</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>20000</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <v>22000</v>
       </c>
-      <c r="I2" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J2" s="0" t="s">
+      <c r="L2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="V2" s="1" t="n">
+        <v>199.99</v>
+      </c>
+      <c r="W2" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="R2" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="S2" s="0" t="n">
-        <v>199.99</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2304,17 +2331,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2325,60 +2355,54 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2390,67 +2414,61 @@
         <v>24</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>60000</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="G2" s="3" t="n">
         <v>44959</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="H2" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="I2" s="2" t="n">
         <v>5000</v>
       </c>
-      <c r="H2" s="2" t="n">
-        <v>3000</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>900</v>
-      </c>
       <c r="J2" s="2" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="K2" s="2" t="n">
         <v>2000</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="M2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="P2" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="P2" s="2" t="n">
-        <v>1</v>
-      </c>
       <c r="Q2" s="2" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="R2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="S2" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T2" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2463,13 +2481,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2479,39 +2502,60 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2522,41 +2566,62 @@
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="E2" s="3" t="n">
         <v>44959</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="F2" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="G2" s="2" t="n">
         <v>5000</v>
       </c>
-      <c r="G2" s="2" t="n">
-        <v>1000</v>
-      </c>
       <c r="H2" s="2" t="n">
-        <v>20</v>
+        <v>3000</v>
       </c>
       <c r="I2" s="2" t="n">
+        <v>900</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="J2" s="2" t="n">
-        <v>400</v>
-      </c>
-      <c r="K2" s="2" t="n">
+      <c r="L2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="M2" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>87</v>
+      <c r="P2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2575,13 +2640,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2606,15 +2671,24 @@
         <v>76</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2641,15 +2715,24 @@
         <v>1000</v>
       </c>
       <c r="H2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="J2" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="K2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="J2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2669,13 +2752,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2700,24 +2783,15 @@
         <v>76</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2744,25 +2818,16 @@
         <v>1000</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>400</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="M2" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>56</v>
+        <v>5</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2781,80 +2846,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="2" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="25.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="2" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="T1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2865,65 +2905,47 @@
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
+      <c r="C2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>44959</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>20000</v>
+        <v>1000</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>6000</v>
+        <v>400</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>199.99</v>
-      </c>
-      <c r="N2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="Q2" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>82</v>
+        <v>20</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2936,13 +2958,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="2" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="25.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="2" width="11.52"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2961,42 +2990,48 @@
         <v>63</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3017,43 +3052,49 @@
         <v>100</v>
       </c>
       <c r="F2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" s="2" t="n">
         <v>20000</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="J2" s="2" t="n">
         <v>6000</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="K2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="J2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="K2" s="2" t="n">
+      <c r="L2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M2" s="2" t="n">
         <v>199.99</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="O2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q2" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="2" t="n">
+      <c r="R2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>87</v>
+      <c r="T2" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3074,11 +3115,11 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -3174,7 +3215,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>0</v>
@@ -3183,13 +3224,13 @@
         <v>200</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3208,20 +3249,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="2" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="25.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="2" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -3240,48 +3274,42 @@
         <v>63</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>91</v>
+      <c r="G1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="S1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3302,49 +3330,43 @@
         <v>100</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>100</v>
+        <v>20000</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="H2" s="2" t="n">
+        <v>6000</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>199.99</v>
+      </c>
+      <c r="L2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" s="2" t="n">
-        <v>10000</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>6000</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M2" s="2" t="n">
-        <v>199.99</v>
+      <c r="M2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="2" t="n">
-        <v>0.2</v>
+      <c r="O2" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3363,18 +3385,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="2" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="27.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="2" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="25.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="2" width="11.52"/>
   </cols>
   <sheetData>
@@ -3395,42 +3417,48 @@
         <v>63</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3451,43 +3479,49 @@
         <v>100</v>
       </c>
       <c r="F2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" s="2" t="n">
         <v>20000</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="J2" s="2" t="n">
         <v>6000</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="K2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="J2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="K2" s="2" t="n">
+      <c r="L2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M2" s="2" t="n">
         <v>199.99</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="O2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q2" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="2" t="n">
+      <c r="R2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>56</v>
+      <c r="T2" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3506,18 +3540,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="2" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="25.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="2" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="27.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="2" width="11.52"/>
   </cols>
   <sheetData>
@@ -3538,48 +3572,42 @@
         <v>63</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>91</v>
+      <c r="G1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="S1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3600,48 +3628,42 @@
         <v>100</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>100</v>
+        <v>20000</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="H2" s="2" t="n">
+        <v>6000</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>199.99</v>
+      </c>
+      <c r="L2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" s="2" t="n">
-        <v>10000</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>6000</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M2" s="2" t="n">
-        <v>199.99</v>
+      <c r="M2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="2" t="n">
-        <v>0.2</v>
+      <c r="O2" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3663,11 +3685,11 @@
   </sheetPr>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="0" width="23.08"/>
   </cols>
@@ -3763,10 +3785,10 @@
         <v>1000</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>100</v>
@@ -3812,46 +3834,80 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="2" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="25.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="2" width="11.52"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3862,38 +3918,65 @@
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>44959</v>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>5000</v>
+        <v>100</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>6000</v>
+      </c>
+      <c r="K2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="I2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>199.99</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3906,13 +3989,107 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>44959</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="14.35"/>
@@ -4016,7 +4193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4027,7 +4204,7 @@
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="0" width="23.08"/>
   </cols>
@@ -4123,7 +4300,7 @@
         <v>1000</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>26</v>
@@ -4153,7 +4330,7 @@
         <v>199.99</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -4174,11 +4351,11 @@
   </sheetPr>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="0" width="23.08"/>
   </cols>
@@ -4274,10 +4451,10 @@
         <v>1000</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>100</v>
@@ -4323,165 +4500,145 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="0" width="23.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="W1" s="2" t="s">
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>44959</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>3000</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>900</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="n">
+      <c r="C2" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>630</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>22000</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="L2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="M2" s="2" t="n">
+      <c r="O2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="P2" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="N2" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="P2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="R2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="T2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U2" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="V2" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>56</v>
+      <c r="Q2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>199.99</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4496,11 +4653,11 @@
   </sheetPr>
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.83"/>
@@ -4607,7 +4764,7 @@
         <v>900</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2" s="2" t="n">
         <v>2000</v>
@@ -4652,7 +4809,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4665,17 +4822,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4707,16 +4864,16 @@
         <v>40</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>45</v>
@@ -4725,21 +4882,27 @@
         <v>46</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -4772,14 +4935,16 @@
         <v>900</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="K2" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>2000</v>
+      </c>
       <c r="L2" s="2" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>100</v>
@@ -4788,28 +4953,34 @@
         <v>55</v>
       </c>
       <c r="P2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="R2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="Q2" s="2" t="n">
+      <c r="S2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="R2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="S2" s="2" t="n">
+      <c r="T2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U2" s="2" t="n">
         <v>600</v>
       </c>
-      <c r="T2" s="2" t="n">
+      <c r="V2" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4825,10 +4996,10 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
@@ -4966,7 +5137,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4981,13 +5152,13 @@
   </sheetPr>
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
   </cols>
@@ -5021,22 +5192,22 @@
         <v>40</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>49</v>
@@ -5085,21 +5256,21 @@
       <c r="I2" s="2" t="n">
         <v>900</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="n">
+      <c r="J2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="L2" s="2" t="n">
-        <v>1000</v>
-      </c>
       <c r="M2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N2" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="O2" s="2" t="n">
-        <v>2</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>1</v>

</xml_diff>